<commit_message>
added kernel and main and now 1 works, 2.1 is written and the arrays gridStart gridEnd are working correctly
</commit_message>
<xml_diff>
--- a/profileResults.xlsx
+++ b/profileResults.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20000" windowHeight="11247"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20000" windowHeight="11247" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>run statistics</t>
   </si>
@@ -66,12 +66,21 @@
   </si>
   <si>
     <t>same as above</t>
+  </si>
+  <si>
+    <t>dt</t>
+  </si>
+  <si>
+    <t>too few to join boids stuck</t>
+  </si>
+  <si>
+    <t>enough to run and the boids merge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,16 +425,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,7 +442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -453,13 +462,16 @@
         <v>5</v>
       </c>
       <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -479,13 +491,16 @@
         <v>10000</v>
       </c>
       <c r="G3">
+        <v>0.2</v>
+      </c>
+      <c r="H3">
         <v>26</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -505,13 +520,59 @@
         <v>10000</v>
       </c>
       <c r="G4">
+        <v>0.2</v>
+      </c>
+      <c r="H4">
         <v>26</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>12</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+      <c r="G5">
+        <v>0.4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
+      </c>
+      <c r="H6">
+        <v>107</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scattered working and coherent is written and compiling
</commit_message>
<xml_diff>
--- a/profileResults.xlsx
+++ b/profileResults.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>run statistics</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>enough to run and the boids merge</t>
+  </si>
+  <si>
+    <t>naïve test release same as before</t>
+  </si>
+  <si>
+    <t>scattered</t>
   </si>
 </sst>
 </file>
@@ -426,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -575,6 +581,52 @@
         <v>16</v>
       </c>
     </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
+      <c r="F7">
+        <v>10000</v>
+      </c>
+      <c r="G7">
+        <v>0.2</v>
+      </c>
+      <c r="H7">
+        <v>26</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>10000</v>
+      </c>
+      <c r="G8">
+        <v>0.2</v>
+      </c>
+      <c r="H8">
+        <v>108.2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>